<commit_message>
Changes made to run on local. Revert back after development
</commit_message>
<xml_diff>
--- a/admin/payslip_data.xlsx
+++ b/admin/payslip_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -59,67 +59,61 @@
     <t>MANJHI</t>
   </si>
   <si>
-    <t xml:space="preserve">600  </t>
-  </si>
-  <si>
-    <t>2024-03-29 16:04:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOM </t>
-  </si>
-  <si>
-    <t>MARANDI</t>
-  </si>
-  <si>
-    <t>2024-03-29 16:15:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUKHIN </t>
-  </si>
-  <si>
-    <t>2024-03-29 16:16:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DHARMENDRA </t>
-  </si>
-  <si>
-    <t>HEMBROM</t>
-  </si>
-  <si>
-    <t>2024-03-29 16:17:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIJAY </t>
-  </si>
-  <si>
-    <t>2024-03-29 16:17:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIVDHAN </t>
-  </si>
-  <si>
-    <t>BASKI</t>
-  </si>
-  <si>
-    <t>2024-03-29 16:18:24</t>
-  </si>
-  <si>
-    <t>SURESH</t>
-  </si>
-  <si>
-    <t>SOREN</t>
-  </si>
-  <si>
-    <t>2024-03-29 16:18:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEVENDRA </t>
-  </si>
-  <si>
-    <t>MARIK</t>
-  </si>
-  <si>
-    <t>2024-03-29 16:19:23</t>
+    <t>2024-03-04 08:58:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROBIN </t>
+  </si>
+  <si>
+    <t>MANDAL</t>
+  </si>
+  <si>
+    <t>2024-03-04 09:04:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KALI </t>
+  </si>
+  <si>
+    <t>TUDU</t>
+  </si>
+  <si>
+    <t>2024-03-14 14:54:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEPAL </t>
+  </si>
+  <si>
+    <t>MAHTO</t>
+  </si>
+  <si>
+    <t>2024-03-14 15:51:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANSHI </t>
+  </si>
+  <si>
+    <t>2024-03-14 16:00:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAJESH </t>
+  </si>
+  <si>
+    <t>ROSHAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600 </t>
+  </si>
+  <si>
+    <t>2024-03-20 22:28:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nassour </t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>2024-03-24 18:09:58</t>
   </si>
 </sst>
 </file>
@@ -496,7 +490,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:M1"/>
@@ -545,7 +539,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -553,105 +547,101 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
+      <c r="D2">
+        <v>600</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F2">
-        <v>9000</v>
+        <v>13800</v>
       </c>
       <c r="G2">
         <v>2400.0</v>
       </c>
       <c r="H2">
-        <v>1200.0</v>
+        <v>5000.0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>3000.0</v>
       </c>
       <c r="J2">
         <v>1200.0</v>
       </c>
       <c r="K2">
-        <v>4700</v>
+        <v>2600</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>500</v>
-      </c>
+      <c r="D3"/>
       <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3">
-        <v>15000</v>
-      </c>
+      <c r="F3"/>
       <c r="G3">
-        <v>1400.0</v>
+        <v>1200.0</v>
       </c>
       <c r="H3">
-        <v>3000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="I3">
-        <v>4000.0</v>
+        <v>2000.0</v>
       </c>
       <c r="J3">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
       <c r="K3">
-        <v>5400</v>
+        <v>-10600</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>-10</v>
       </c>
       <c r="F4">
-        <v>12500</v>
+        <v>7000</v>
       </c>
       <c r="G4">
-        <v>2400.0</v>
+        <v>21.0</v>
       </c>
       <c r="H4">
-        <v>1000.0</v>
+        <v>211.0</v>
       </c>
       <c r="I4">
-        <v>2000.0</v>
+        <v>21.0</v>
       </c>
       <c r="J4">
-        <v>2000.0</v>
+        <v>12.0</v>
       </c>
       <c r="K4">
-        <v>5600</v>
+        <v>6851.6666666667</v>
       </c>
       <c r="L4" t="s">
         <v>20</v>
@@ -659,7 +649,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -668,28 +658,28 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F5">
-        <v>6000</v>
+        <v>24000</v>
       </c>
       <c r="G5">
         <v>2400.0</v>
       </c>
       <c r="H5">
-        <v>2000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="I5">
-        <v>7000.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J5">
-        <v>2000.0</v>
+        <v>1200.0</v>
       </c>
       <c r="K5">
-        <v>-10900</v>
+        <v>15933.333333333</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
@@ -697,37 +687,37 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="E6">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6">
-        <v>16800</v>
+        <v>21000</v>
       </c>
       <c r="G6">
-        <v>2400.0</v>
+        <v>3200.0</v>
       </c>
       <c r="H6">
-        <v>1400.0</v>
+        <v>1000.0</v>
       </c>
       <c r="I6">
-        <v>3000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J6">
         <v>1200.0</v>
       </c>
       <c r="K6">
-        <v>8800</v>
+        <v>12566.666666667</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
@@ -735,7 +725,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -743,108 +733,70 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
-        <v>600</v>
+      <c r="D7" t="s">
+        <v>28</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F7">
-        <v>13800</v>
+        <v>15000.0</v>
       </c>
       <c r="G7">
-        <v>0.0</v>
+        <v>1200.0</v>
       </c>
       <c r="H7">
         <v>1000.0</v>
       </c>
       <c r="I7">
-        <v>2000.0</v>
+        <v>7000.0</v>
       </c>
       <c r="J7">
-        <v>1200.0</v>
+        <v>1000.0</v>
       </c>
       <c r="K7">
-        <v>9600</v>
+        <v>5090.0</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>123</v>
+      </c>
+      <c r="E8">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <v>500</v>
-      </c>
-      <c r="E8">
-        <v>26</v>
-      </c>
       <c r="F8">
-        <v>13000</v>
+        <v>2460</v>
       </c>
       <c r="G8">
-        <v>2400.0</v>
+        <v>2.0</v>
       </c>
       <c r="H8">
-        <v>2000.0</v>
+        <v>2.0</v>
       </c>
       <c r="I8">
-        <v>1200.0</v>
+        <v>2.0</v>
       </c>
       <c r="J8">
-        <v>1200.0</v>
+        <v>2.0</v>
       </c>
       <c r="K8">
-        <v>3800</v>
+        <v>2472.5</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>550</v>
-      </c>
-      <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>16500</v>
-      </c>
-      <c r="G9">
-        <v>2400.0</v>
-      </c>
-      <c r="H9">
-        <v>4000.0</v>
-      </c>
-      <c r="I9">
-        <v>4000.0</v>
-      </c>
-      <c r="J9">
-        <v>1200.0</v>
-      </c>
-      <c r="K9">
-        <v>5816.6666666667</v>
-      </c>
-      <c r="L9" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>